<commit_message>
Tidy up naming of documents
Tidy up naming of documents
</commit_message>
<xml_diff>
--- a/schedule/G6T6 Shared Timetable.xlsx
+++ b/schedule/G6T6 Shared Timetable.xlsx
@@ -1,21 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\project-g6t6\schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BA1F16-DBBE-4747-87DE-4C204BFDECFD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F80ACD7-0373-4D3C-B601-0254F51AF02B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -49,10 +57,6 @@
     <t>BPAS(SJ)</t>
   </si>
   <si>
-    <t>CT(SJ,ZC)
-IDP (M)</t>
-  </si>
-  <si>
     <t>BPAS (S)
 BPAS (ZY) 
 IDP(SJ)</t>
@@ -85,9 +89,6 @@
     <t>3.30 - 6.45</t>
   </si>
   <si>
-    <t>wad(sj)</t>
-  </si>
-  <si>
     <t>CTRW(ZY)
 CT (M)</t>
   </si>
@@ -147,6 +148,12 @@
   </si>
   <si>
     <t>SH</t>
+  </si>
+  <si>
+    <t>WAD (SJ)</t>
+  </si>
+  <si>
+    <t>CT(SJ,ZC)</t>
   </si>
 </sst>
 </file>
@@ -343,12 +350,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -374,13 +375,19 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -603,417 +610,410 @@
   </sheetPr>
   <dimension ref="A1:AR13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA4" sqref="AA4"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+      <selection activeCell="AO16" sqref="AO16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="1"/>
-    <col min="2" max="2" width="3.6640625" customWidth="1"/>
-    <col min="3" max="3" width="3.33203125" customWidth="1"/>
-    <col min="4" max="5" width="3.5546875" customWidth="1"/>
-    <col min="6" max="7" width="3.6640625" customWidth="1"/>
-    <col min="8" max="8" width="3.33203125" customWidth="1"/>
-    <col min="9" max="10" width="3.5546875" customWidth="1"/>
-    <col min="11" max="12" width="3.6640625" customWidth="1"/>
-    <col min="13" max="14" width="3.5546875" customWidth="1"/>
-    <col min="15" max="17" width="3.6640625" customWidth="1"/>
-    <col min="18" max="18" width="3.33203125" customWidth="1"/>
-    <col min="19" max="20" width="3.5546875" customWidth="1"/>
-    <col min="21" max="22" width="3.6640625" customWidth="1"/>
-    <col min="23" max="23" width="3.33203125" customWidth="1"/>
-    <col min="24" max="25" width="3.5546875" customWidth="1"/>
-    <col min="26" max="27" width="3.6640625" customWidth="1"/>
-    <col min="28" max="28" width="3.33203125" customWidth="1"/>
-    <col min="29" max="30" width="3.5546875" customWidth="1"/>
-    <col min="31" max="32" width="3.6640625" customWidth="1"/>
-    <col min="33" max="33" width="3.33203125" customWidth="1"/>
-    <col min="34" max="35" width="3.5546875" customWidth="1"/>
-    <col min="36" max="36" width="3.6640625" customWidth="1"/>
-    <col min="37" max="37" width="10.88671875" customWidth="1"/>
-    <col min="38" max="38" width="11.44140625" customWidth="1"/>
-    <col min="39" max="39" width="9.44140625" customWidth="1"/>
-    <col min="40" max="40" width="10.88671875" customWidth="1"/>
-    <col min="41" max="41" width="10" customWidth="1"/>
-    <col min="42" max="42" width="10.109375" customWidth="1"/>
-    <col min="43" max="43" width="8.5546875" customWidth="1"/>
-    <col min="44" max="44" width="7.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="3.6640625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="3.33203125" hidden="1" customWidth="1"/>
+    <col min="4" max="5" width="3.5546875" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="3.6640625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="3.33203125" hidden="1" customWidth="1"/>
+    <col min="9" max="10" width="3.5546875" hidden="1" customWidth="1"/>
+    <col min="11" max="12" width="3.6640625" hidden="1" customWidth="1"/>
+    <col min="13" max="14" width="3.5546875" hidden="1" customWidth="1"/>
+    <col min="15" max="17" width="3.6640625" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="3.33203125" hidden="1" customWidth="1"/>
+    <col min="19" max="20" width="3.5546875" hidden="1" customWidth="1"/>
+    <col min="21" max="22" width="3.6640625" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="3.33203125" hidden="1" customWidth="1"/>
+    <col min="24" max="25" width="3.5546875" hidden="1" customWidth="1"/>
+    <col min="26" max="27" width="3.6640625" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="3.33203125" hidden="1" customWidth="1"/>
+    <col min="29" max="30" width="3.5546875" hidden="1" customWidth="1"/>
+    <col min="31" max="32" width="3.6640625" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="3.33203125" hidden="1" customWidth="1"/>
+    <col min="34" max="35" width="3.5546875" hidden="1" customWidth="1"/>
+    <col min="36" max="36" width="3.6640625" hidden="1" customWidth="1"/>
+    <col min="37" max="44" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-      <c r="B1" s="26" t="s">
+      <c r="A1" s="3"/>
+      <c r="B1" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="29" t="s">
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="29" t="s">
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="29" t="s">
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="29" t="s">
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="26"/>
+      <c r="AF1" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="28"/>
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="25"/>
+      <c r="AI1" s="25"/>
+      <c r="AJ1" s="26"/>
     </row>
     <row r="2" spans="1:44" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
+      <c r="A2" s="4"/>
       <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q2" s="8" t="s">
+      <c r="Q2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="U2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="V2" s="8" t="s">
+      <c r="V2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Z2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="Y2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA2" s="8" t="s">
+      <c r="AA2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AE2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AD2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE2" s="7" t="s">
-        <v>37</v>
-      </c>
       <c r="AF2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AJ2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AI2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AJ2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="AK2" s="2"/>
-      <c r="AL2" s="3" t="s">
+      <c r="AK2" s="28"/>
+      <c r="AL2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="AM2" s="3" t="s">
+      <c r="AM2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="AN2" s="3" t="s">
+      <c r="AN2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="AO2" s="3" t="s">
+      <c r="AO2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="AP2" s="3" t="s">
+      <c r="AP2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="AQ2" s="3" t="s">
+      <c r="AQ2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="AR2" s="3" t="s">
+      <c r="AR2" s="28" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:44" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="14"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="15"/>
-      <c r="V3" s="13"/>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
-      <c r="Z3" s="17"/>
-      <c r="AA3" s="13"/>
-      <c r="AE3" s="15"/>
-      <c r="AJ3" s="15"/>
-      <c r="AK3" s="3" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="12"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="12"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="12"/>
+      <c r="X3" s="12"/>
+      <c r="Z3" s="15"/>
+      <c r="AA3" s="11"/>
+      <c r="AE3" s="13"/>
+      <c r="AJ3" s="13"/>
+      <c r="AK3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="AL3" s="2"/>
-      <c r="AM3" s="3" t="s">
+      <c r="AL3" s="28"/>
+      <c r="AM3" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="AN3" s="2"/>
-      <c r="AO3" s="3" t="s">
+      <c r="AN3" s="28"/>
+      <c r="AO3" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="AP3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AQ3" s="2"/>
-      <c r="AR3" s="2"/>
+      <c r="AQ3" s="28"/>
+      <c r="AR3" s="28"/>
     </row>
     <row r="4" spans="1:44" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="11"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="14"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="14"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="13"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="11"/>
+      <c r="AE4" s="13"/>
+      <c r="AJ4" s="13"/>
+      <c r="AK4" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL4" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="13"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="16"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="16"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="11"/>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="11"/>
-      <c r="Z4" s="12"/>
-      <c r="AA4" s="13"/>
-      <c r="AE4" s="15"/>
-      <c r="AJ4" s="15"/>
-      <c r="AK4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="AL4" s="3" t="s">
+      <c r="AM4" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="AM4" s="3" t="s">
+      <c r="AN4" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="AN4" s="3" t="s">
+      <c r="AO4" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="AO4" s="3" t="s">
+      <c r="AP4" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="AP4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="AQ4" s="2"/>
-      <c r="AR4" s="2"/>
+      <c r="AQ4" s="28"/>
+      <c r="AR4" s="28"/>
     </row>
     <row r="5" spans="1:44" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="14"/>
+      <c r="N5" s="12"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="14"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="10"/>
+      <c r="AA5" s="11"/>
+      <c r="AE5" s="13"/>
+      <c r="AJ5" s="13"/>
+      <c r="AK5" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL5" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM5" s="28"/>
+      <c r="AN5" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="16"/>
-      <c r="N5" s="14"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="16"/>
-      <c r="U5" s="17"/>
-      <c r="V5" s="10"/>
-      <c r="W5" s="11"/>
-      <c r="X5" s="11"/>
-      <c r="Y5" s="11"/>
-      <c r="Z5" s="12"/>
-      <c r="AA5" s="13"/>
-      <c r="AE5" s="15"/>
-      <c r="AJ5" s="15"/>
-      <c r="AK5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="AL5" s="3" t="s">
+      <c r="AO5" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="AM5" s="2"/>
-      <c r="AN5" s="3" t="s">
+      <c r="AP5" s="28"/>
+      <c r="AQ5" s="28"/>
+      <c r="AR5" s="28"/>
+    </row>
+    <row r="6" spans="1:44" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AO5" s="3" t="s">
+      <c r="B6" s="16"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="17"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="17"/>
+      <c r="X6" s="17"/>
+      <c r="Y6" s="17"/>
+      <c r="Z6" s="19"/>
+      <c r="AA6" s="20"/>
+      <c r="AB6" s="17"/>
+      <c r="AC6" s="17"/>
+      <c r="AD6" s="17"/>
+      <c r="AE6" s="19"/>
+      <c r="AF6" s="17"/>
+      <c r="AG6" s="17"/>
+      <c r="AH6" s="17"/>
+      <c r="AI6" s="17"/>
+      <c r="AJ6" s="19"/>
+      <c r="AK6" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="AL6" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="AP5" s="2"/>
-      <c r="AQ5" s="2"/>
-      <c r="AR5" s="2"/>
-    </row>
-    <row r="6" spans="1:44" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="AM6" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="19"/>
-      <c r="S6" s="19"/>
-      <c r="T6" s="19"/>
-      <c r="U6" s="21"/>
-      <c r="V6" s="18"/>
-      <c r="W6" s="19"/>
-      <c r="X6" s="19"/>
-      <c r="Y6" s="19"/>
-      <c r="Z6" s="21"/>
-      <c r="AA6" s="22"/>
-      <c r="AB6" s="19"/>
-      <c r="AC6" s="19"/>
-      <c r="AD6" s="19"/>
-      <c r="AE6" s="21"/>
-      <c r="AF6" s="19"/>
-      <c r="AG6" s="19"/>
-      <c r="AH6" s="19"/>
-      <c r="AI6" s="19"/>
-      <c r="AJ6" s="21"/>
-      <c r="AK6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="AL6" s="3" t="s">
+      <c r="AN6" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="AM6" s="3" t="s">
+      <c r="AO6" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="AN6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="AO6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AP6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AQ6" s="2"/>
-      <c r="AR6" s="2"/>
+      <c r="AP6" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="AQ6" s="28"/>
+      <c r="AR6" s="28"/>
     </row>
     <row r="7" spans="1:44" ht="13.2" x14ac:dyDescent="0.25">
       <c r="AK7" s="1"/>
@@ -1040,7 +1040,7 @@
     <row r="11" spans="1:44" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:44" ht="13.2" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:44" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="K13" s="25"/>
+      <c r="K13" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>